<commit_message>
Updated Timestamp for Level 1
Commited saved saved changes
</commit_message>
<xml_diff>
--- a/assets/lvl2timestamp.xlsx
+++ b/assets/lvl2timestamp.xlsx
@@ -337,10 +337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A117"/>
+  <dimension ref="A1:A121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,6 +933,26 @@
         <v>51.1</v>
       </c>
     </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>51.3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>51.7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>51.9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>52.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>